<commit_message>
Change Variables excel file
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara1\GitHub\IND5003-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC97C03-EE25-4518-AC7B-27828EA7482B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1390D83-35D4-4468-BD8B-81E89AEF7988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>RXDCOUNT</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>LBXGH</t>
+  </si>
+  <si>
+    <t>VAR</t>
   </si>
 </sst>
 </file>
@@ -608,11 +611,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716A7EE8-5A97-4A9E-B2AD-A8EFFA1D3E8E}">
-  <dimension ref="A1:A78"/>
+  <dimension ref="A1:A79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -621,391 +622,396 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created base dataset from 75 Variables
Edits also made to Variables file:
1) "PHAFSTMN" to "PHAFSTMN.x" because that is how it is coded in the lab dataset

2) "LBXVIDMS" removed as this is not found in lab dataset
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara1\GitHub\IND5003-Group-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\Documents\GitHub\IND5003-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1390D83-35D4-4468-BD8B-81E89AEF7988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2A2DA-8DA0-4E19-A337-E02C1589CF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>RXDCOUNT</t>
   </si>
@@ -81,9 +81,6 @@
     <t>DR1TALCO</t>
   </si>
   <si>
-    <t>DR1_320Z</t>
-  </si>
-  <si>
     <t>LBDGLTSI</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>WHQ030</t>
   </si>
   <si>
-    <t>PHAFSTMN</t>
-  </si>
-  <si>
     <t>LBDHDDSI</t>
   </si>
   <si>
@@ -252,13 +246,16 @@
     <t>LBXIN</t>
   </si>
   <si>
-    <t>LBXVIDMS</t>
-  </si>
-  <si>
     <t>LBXGH</t>
   </si>
   <si>
     <t>VAR</t>
+  </si>
+  <si>
+    <t>DR1.320Z</t>
+  </si>
+  <si>
+    <t>PHAFSTMN.x</t>
   </si>
 </sst>
 </file>
@@ -611,407 +608,399 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716A7EE8-5A97-4A9E-B2AD-A8EFFA1D3E8E}">
-  <dimension ref="A1:A79"/>
+  <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A45" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A47" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A48" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A52" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A53" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A54" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A55" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A56" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A57" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A58" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A60" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A61" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A62" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A63" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A64" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A66" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A70" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A71" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A74" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A78" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 1 Variable, Added Wes working file
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\Documents\GitHub\IND5003-Group-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tay_w\Documents\GitHub\IND5003-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2A2DA-8DA0-4E19-A337-E02C1589CF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2352DC9F-9026-43EF-A003-ED7EF0A343D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>RXDCOUNT</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>PHAFSTMN.x</t>
+  </si>
+  <si>
+    <t>HSD010</t>
   </si>
 </sst>
 </file>
@@ -608,399 +611,404 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716A7EE8-5A97-4A9E-B2AD-A8EFFA1D3E8E}">
-  <dimension ref="A1:A77"/>
+  <dimension ref="A1:A78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to variables and main
Variables file updated to remove the spacing. Updated main python notebook to include Sara and Wes updates
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara1\GitHub\IND5003-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EA7702-9AFD-477F-BE80-85A3CCDAE925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529DFE0E-2E86-4B83-B71A-60E8FBB62DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
   </bookViews>
@@ -213,22 +213,22 @@
     <t>DR1.320Z</t>
   </si>
   <si>
-    <t xml:space="preserve">LBDHDDSI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LBDTCSI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LBXVIDMS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LBXGH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHQ030 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHQ070 </t>
+    <t>WHQ070</t>
+  </si>
+  <si>
+    <t>WHQ030</t>
+  </si>
+  <si>
+    <t>LBDHDDSI</t>
+  </si>
+  <si>
+    <t>LBDTCSI</t>
+  </si>
+  <si>
+    <t>LBXVIDMS</t>
+  </si>
+  <si>
+    <t>LBXGH</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716A7EE8-5A97-4A9E-B2AD-A8EFFA1D3E8E}">
   <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:XFD66"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -684,22 +684,22 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
@@ -904,12 +904,12 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Variable Files and main notebook
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara1\GitHub\IND5003-Group-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tay_w\Documents\GitHub\IND5003-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529DFE0E-2E86-4B83-B71A-60E8FBB62DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90141F02-F0DB-46BE-BADE-6E191EE1EB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4B6DA73-DEED-49E8-8A55-61AFB6DEB1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>RXDCOUNT</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>LBXGH</t>
+  </si>
+  <si>
+    <t>HSD010</t>
   </si>
 </sst>
 </file>
@@ -581,354 +584,359 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716A7EE8-5A97-4A9E-B2AD-A8EFFA1D3E8E}">
-  <dimension ref="A1:A68"/>
+  <dimension ref="A1:A69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>